<commit_message>
updated unit price for bridal laces
</commit_message>
<xml_diff>
--- a/price list.xlsx
+++ b/price list.xlsx
@@ -32,31 +32,31 @@
     <t>item</t>
   </si>
   <si>
-    <t>organza fabric</t>
-  </si>
-  <si>
     <t>unit price</t>
   </si>
   <si>
     <t>qty</t>
   </si>
   <si>
-    <t>jeans fabric</t>
-  </si>
-  <si>
-    <t>suiting fabric</t>
-  </si>
-  <si>
     <t>lining</t>
   </si>
   <si>
-    <t>bridal lace</t>
-  </si>
-  <si>
-    <t>black dry lace</t>
-  </si>
-  <si>
-    <t>white dry lace</t>
+    <t>organza fabrics</t>
+  </si>
+  <si>
+    <t>jeans fabrics</t>
+  </si>
+  <si>
+    <t>suiting fabrics</t>
+  </si>
+  <si>
+    <t>bridal laces</t>
+  </si>
+  <si>
+    <t>black dry laces</t>
+  </si>
+  <si>
+    <t>white dry laces</t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -394,10 +394,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -405,7 +405,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -427,7 +427,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>50</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -452,7 +452,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D6">
         <v>12</v>

</xml_diff>